<commit_message>
Add SQL script for creating tables
</commit_message>
<xml_diff>
--- a/Lab/Hotel.xlsx
+++ b/Lab/Hotel.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="155">
   <si>
     <t>Gäste</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Vorname</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t>DienstleistungId</t>
-  </si>
-  <si>
-    <t>DienstleistungTyp</t>
   </si>
   <si>
     <t>Preis</t>
@@ -974,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,15 +1000,15 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="J1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -1035,254 +1029,254 @@
         <v>0</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="J6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J7" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J8" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J9" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="J11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1303,93 +1297,93 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1402,187 +1396,187 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1595,608 +1589,608 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C47" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="G48" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C49" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51" s="6" t="s">
+      <c r="B54" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B72" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="G72" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="15" t="s">
+      <c r="B77" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65" s="8" t="s">
+      <c r="C77" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B78" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="8" t="s">
+      <c r="C78" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F67" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G67" s="6" t="s">
+      <c r="D79" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="8" t="s">
+      <c r="E79" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B80" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E68" s="6" t="s">
+      <c r="C80" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="E80" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B69" s="8" t="s">
+      <c r="F80" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F69" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B70" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="F81" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B76" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B77" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B83" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B84" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update create script + add insert script
</commit_message>
<xml_diff>
--- a/Lab/Hotel.xlsx
+++ b/Lab/Hotel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="153">
   <si>
     <t>Gäste</t>
   </si>
@@ -127,9 +127,6 @@
     <t>GesamtBetrag</t>
   </si>
   <si>
-    <t>IstBezahtl</t>
-  </si>
-  <si>
     <t>Dienstleistungen</t>
   </si>
   <si>
@@ -472,13 +469,10 @@
     <t>BZId</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>17-04-2023</t>
+  </si>
+  <si>
+    <t>Leaga de Buchungen</t>
   </si>
 </sst>
 </file>
@@ -494,7 +488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +555,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -611,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -662,6 +662,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -970,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +1003,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="J1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1029,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>8</v>
@@ -1040,57 +1043,57 @@
         <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1098,25 +1101,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>11</v>
@@ -1127,25 +1130,25 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>33</v>
@@ -1153,10 +1156,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J7" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>15</v>
@@ -1167,7 +1170,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>8</v>
@@ -1178,10 +1181,10 @@
         <v>3</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1189,13 +1192,13 @@
         <v>3</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1206,25 +1209,25 @@
         <v>5</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>3</v>
@@ -1235,25 +1238,25 @@
         <v>6</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>15</v>
@@ -1264,19 +1267,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1308,19 +1311,19 @@
         <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1331,19 +1334,19 @@
         <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1351,19 +1354,19 @@
         <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1371,19 +1374,19 @@
         <v>10</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1396,7 +1399,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1404,22 +1407,22 @@
         <v>19</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1430,19 +1433,19 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1453,19 +1456,19 @@
         <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1481,19 +1484,19 @@
         <v>34</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1504,19 +1507,19 @@
         <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1524,19 +1527,19 @@
         <v>35</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1544,40 +1547,28 @@
         <v>36</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>152</v>
-      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
@@ -1600,39 +1591,39 @@
         <v>24</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1640,19 +1631,19 @@
         <v>1</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1660,19 +1651,19 @@
         <v>25</v>
       </c>
       <c r="C43" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1688,19 +1679,19 @@
         <v>21</v>
       </c>
       <c r="C47" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1711,22 +1702,22 @@
         <v>34</v>
       </c>
       <c r="C48" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -1734,135 +1725,135 @@
         <v>24</v>
       </c>
       <c r="C49" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C50" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="E50" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G50" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="E51" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="F51" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="E54" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="F54" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B55" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="E55" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="F55" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="G55" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G55" s="6" t="s">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B56" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="8" t="s">
+      <c r="E56" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -1870,82 +1861,85 @@
         <v>4</v>
       </c>
       <c r="C60" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="E60" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="F60" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="G60" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G60" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I60" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="E61" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="F61" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="G61" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G61" s="6" t="s">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B62" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="6" t="s">
+      <c r="D62" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="E62" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F62" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B63" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C63" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G63" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -1961,19 +1955,19 @@
         <v>12</v>
       </c>
       <c r="C68" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="E68" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="F68" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="G68" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -1984,19 +1978,19 @@
         <v>4</v>
       </c>
       <c r="C69" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="E69" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="F69" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="G69" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2004,22 +1998,22 @@
         <v>20</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="E70" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="F70" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="G70" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2027,19 +2021,19 @@
         <v>13</v>
       </c>
       <c r="C71" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="F71" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2047,19 +2041,19 @@
         <v>14</v>
       </c>
       <c r="C72" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="E72" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="F72" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G72" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2075,19 +2069,19 @@
         <v>28</v>
       </c>
       <c r="C76" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="E76" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="F76" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="G76" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2098,19 +2092,19 @@
         <v>5</v>
       </c>
       <c r="C77" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D77" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="E77" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="F77" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F77" s="6" t="s">
+      <c r="G77" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -2118,19 +2112,19 @@
         <v>29</v>
       </c>
       <c r="C78" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="E78" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="F78" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="G78" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2138,19 +2132,19 @@
         <v>30</v>
       </c>
       <c r="C79" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D79" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="E79" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="F79" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="G79" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -2158,19 +2152,19 @@
         <v>31</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D80" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="F80" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="G80" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
@@ -2178,19 +2172,19 @@
         <v>32</v>
       </c>
       <c r="C81" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D81" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="F81" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="F81" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="G81" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>